<commit_message>
topbar + malo css
</commit_message>
<xml_diff>
--- a/mysite/main/scraping/AkPocasi.xlsx
+++ b/mysite/main/scraping/AkPocasi.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 25.7 °C</t>
+          <t xml:space="preserve"> 24.5 °C</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 40 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,17 +515,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.1 °C</t>
+          <t xml:space="preserve"> 26 °C</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 27 °C</t>
+          <t xml:space="preserve"> 29 °C</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,17 +547,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 24.4 °C</t>
+          <t xml:space="preserve"> 24.2 °C</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 25 °C</t>
+          <t xml:space="preserve"> 27 °C</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 48 %</t>
+          <t xml:space="preserve"> 46 %</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -579,17 +579,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 25 °C</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 26 °C</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 26 °C</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 39 %</t>
+          <t xml:space="preserve"> 40 %</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,17 +643,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 24.8 °C</t>
+          <t xml:space="preserve"> 25 °C</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26 °C</t>
+          <t xml:space="preserve"> 25 °C</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38 %</t>
+          <t xml:space="preserve"> 37 %</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 23.5 °C</t>
+          <t xml:space="preserve"> 23 °C</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 51 %</t>
+          <t xml:space="preserve"> 49 %</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -712,12 +712,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 25 °C</t>
+          <t xml:space="preserve"> 26 °C</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 39 %</t>
+          <t xml:space="preserve"> 40 %</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 41 %</t>
+          <t xml:space="preserve"> 40 %</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -771,17 +771,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26 °C</t>
+          <t xml:space="preserve"> 25.6 °C</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 28 °C</t>
+          <t xml:space="preserve"> 27 °C</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 36 %</t>
         </is>
       </c>
     </row>
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 24.6 °C</t>
+          <t xml:space="preserve"> 24.4 °C</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 39 %</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -835,17 +835,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26 °C</t>
+          <t xml:space="preserve"> 25.6 °C</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 28 °C</t>
+          <t xml:space="preserve"> 27 °C</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 36 %</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 23.5 °C</t>
+          <t xml:space="preserve"> 22.8 °C</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -899,17 +899,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.3 °C</t>
+          <t xml:space="preserve"> 25.8 °C</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 29 °C</t>
+          <t xml:space="preserve"> 28 °C</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 40 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 °C</t>
+          <t xml:space="preserve"> 19 °C</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 44 %</t>
+          <t xml:space="preserve"> 42 %</t>
         </is>
       </c>
     </row>
@@ -953,7 +953,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:49</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -963,17 +963,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26 °C</t>
+          <t xml:space="preserve"> 25.6 °C</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 28 °C</t>
+          <t xml:space="preserve"> 27 °C</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 36 %</t>
         </is>
       </c>
     </row>
@@ -985,7 +985,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:50</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -995,17 +995,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 23 °C</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 24 °C</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 26 °C</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 54 %</t>
+          <t xml:space="preserve"> 52 %</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:50</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1027,17 +1027,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.1 °C</t>
+          <t xml:space="preserve"> 26 °C</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26 °C</t>
+          <t xml:space="preserve"> 28 °C</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15:50</t>
+          <t xml:space="preserve"> 16:43</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1059,17 +1059,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 26.1 °C</t>
+          <t xml:space="preserve"> 26 °C</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 28 °C</t>
+          <t xml:space="preserve"> 29 °C</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 37 %</t>
+          <t xml:space="preserve"> 41 %</t>
         </is>
       </c>
     </row>

</xml_diff>